<commit_message>
add more source data, implement more for view game
</commit_message>
<xml_diff>
--- a/datafiles/GameResult(team).xlsx
+++ b/datafiles/GameResult(team).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Goals scored</t>
   </si>
@@ -75,6 +75,12 @@
   <si>
     <t>Liverpool</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Paris</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -609,6 +615,106 @@
       </c>
       <c r="P3" s="1">
         <v>498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>59</v>
+      </c>
+      <c r="E4" s="1">
+        <v>12</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>1</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>12</v>
+      </c>
+      <c r="N4" s="1">
+        <v>12</v>
+      </c>
+      <c r="O4" s="1">
+        <v>660</v>
+      </c>
+      <c r="P4" s="1">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1">
+        <v>41</v>
+      </c>
+      <c r="E5" s="1">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1">
+        <v>3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>3</v>
+      </c>
+      <c r="K5" s="1">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>12</v>
+      </c>
+      <c r="N5" s="1">
+        <v>11</v>
+      </c>
+      <c r="O5" s="1">
+        <v>430</v>
+      </c>
+      <c r="P5" s="1">
+        <v>387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>